<commit_message>
Clusters names were updated.
</commit_message>
<xml_diff>
--- a/Data/DataFrame_Customers_with_Cluster.xlsx
+++ b/Data/DataFrame_Customers_with_Cluster.xlsx
@@ -8,28 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\DataEnrichment\Project-4-How_to_Market_New_Cards\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0800DBC6-76A1-4574-8892-59BF515E8CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8001653F-034A-4D0C-BC64-A0DAE3497239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -87,18 +73,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -128,16 +108,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,46 +420,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:I854"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18" style="2" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="13.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -22589,16 +22564,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88A2FE7-E8DC-4C37-92E0-10005D086883}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>